<commit_message>
export benchmark results to png
</commit_message>
<xml_diff>
--- a/results/intro_sort_vs_std_sort.xlsx
+++ b/results/intro_sort_vs_std_sort.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://her169626-my.sharepoint.com/personal/f_kretke_otto-hahn-gymnasium_de/Documents/Schule/Facharbeit/facharbeit/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_AD4DB114E441178AC67DF4526E55E246693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53ADAD7F-4D01-43A2-9544-CA0E433ECE19}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_AD4DB114E441178AC67DF4526E55E246693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C5B8DDB-758B-4DD5-9DF9-036A420B20AF}"/>
   <bookViews>
-    <workbookView xWindow="7110" yWindow="2760" windowWidth="33270" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -112,19 +112,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="95000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -150,19 +144,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
@@ -193,19 +181,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -304,19 +286,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -415,19 +391,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -526,19 +496,13 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="34925" cap="rnd">
+            <a:ln w="28575" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+            <a:effectLst/>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
@@ -648,10 +612,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -679,10 +644,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -702,9 +668,9 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="95000"/>
-                <a:alpha val="10000"/>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -718,8 +684,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -748,9 +715,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                  <a:alpha val="10000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -765,10 +732,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="85000"/>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
@@ -778,13 +746,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE"/>
-                  <a:t>Zeit in</a:t>
+                  <a:t>Zeit in ns</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="de-DE" baseline="0"/>
-                  <a:t> ns</a:t>
-                </a:r>
-                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -801,10 +764,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
@@ -834,8 +798,9 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -875,8 +840,9 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -900,28 +866,17 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="dk1">
-            <a:lumMod val="85000"/>
-            <a:lumOff val="15000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln>
-      <a:noFill/>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -984,33 +939,35 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1018,34 +975,26 @@
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill flip="none" rotWithShape="1">
-        <a:gsLst>
-          <a:gs pos="0">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="65000"/>
-              <a:lumOff val="35000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="100000">
-            <a:schemeClr val="dk1">
-              <a:lumMod val="85000"/>
-              <a:lumOff val="15000"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:path path="circle">
-          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-        </a:path>
-        <a:tileRect/>
-      </a:gradFill>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
@@ -1054,8 +1003,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1074,6 +1024,14 @@
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1082,35 +1040,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1122,29 +1090,31 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -1162,18 +1132,21 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1183,20 +1156,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1210,44 +1183,18 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
+  </cs:dropLine>
+  <cs:errorBar>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1257,16 +1204,16 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="10000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
+  </cs:errorBar>
+  <cs:floor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1274,139 +1221,158 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:noFill/>
       <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="5000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
   </cs:seriesLine>
   <cs:title>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="95000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:defRPr>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1422,6 +1388,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1430,8 +1397,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1441,7 +1409,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1449,9 +1417,9 @@
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="54000"/>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1462,8 +1430,9 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1475,6 +1444,12 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1518,10 +1493,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1790,7 +1761,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>